<commit_message>
Update analysis to include has_ad column and make figures highlighting wiht and without AD
</commit_message>
<xml_diff>
--- a/01_raw_data/Moore2023_SI-data.xlsx
+++ b/01_raw_data/Moore2023_SI-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sahar/Documents/methane_letter/01_raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF76BEB3-8E3B-0D43-A46F-28B74832D0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C16419D-A89C-5440-8699-1B908538A2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18800" yWindow="500" windowWidth="19420" windowHeight="21100" activeTab="1" xr2:uid="{07901559-0F47-FB44-87E3-9B6E035880CE}"/>
+    <workbookView xWindow="7260" yWindow="500" windowWidth="30960" windowHeight="23640" activeTab="1" xr2:uid="{07901559-0F47-FB44-87E3-9B6E035880CE}"/>
   </bookViews>
   <sheets>
     <sheet name="tableS4_treatment_categories" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="552">
   <si>
     <t>W005</t>
   </si>
@@ -1669,6 +1669,15 @@
   </si>
   <si>
     <t>ch4_g_per_s_uncertainty</t>
+  </si>
+  <si>
+    <t>has_ad</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -2524,15 +2533,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21717D1-721D-7E42-9C88-DF3348CA9EE9}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A45" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -2548,8 +2557,11 @@
       <c r="E1" s="1" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2565,8 +2577,11 @@
       <c r="E2" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2582,8 +2597,11 @@
       <c r="E3" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -2599,8 +2617,11 @@
       <c r="E4" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -2616,8 +2637,11 @@
       <c r="E5" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2633,8 +2657,11 @@
       <c r="E6" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -2650,8 +2677,11 @@
       <c r="E7" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -2667,8 +2697,11 @@
       <c r="E8" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -2684,8 +2717,11 @@
       <c r="E9" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -2701,8 +2737,11 @@
       <c r="E10" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -2718,8 +2757,11 @@
       <c r="E11" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -2735,8 +2777,11 @@
       <c r="E12" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -2752,8 +2797,11 @@
       <c r="E13" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -2769,8 +2817,11 @@
       <c r="E14" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -2786,8 +2837,11 @@
       <c r="E15" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -2803,8 +2857,11 @@
       <c r="E16" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -2820,8 +2877,11 @@
       <c r="E17" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -2837,8 +2897,11 @@
       <c r="E18" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -2854,8 +2917,11 @@
       <c r="E19" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -2871,8 +2937,11 @@
       <c r="E20" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -2888,8 +2957,11 @@
       <c r="E21" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
@@ -2905,8 +2977,11 @@
       <c r="E22" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -2922,8 +2997,11 @@
       <c r="E23" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>37</v>
       </c>
@@ -2939,8 +3017,11 @@
       <c r="E24" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
@@ -2956,8 +3037,11 @@
       <c r="E25" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
@@ -2973,8 +3057,11 @@
       <c r="E26" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -2990,8 +3077,11 @@
       <c r="E27" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>42</v>
       </c>
@@ -3007,8 +3097,11 @@
       <c r="E28" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
@@ -3024,8 +3117,11 @@
       <c r="E29" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
@@ -3041,8 +3137,11 @@
       <c r="E30" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>45</v>
       </c>
@@ -3058,8 +3157,11 @@
       <c r="E31" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>46</v>
       </c>
@@ -3075,8 +3177,11 @@
       <c r="E32" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>48</v>
       </c>
@@ -3092,8 +3197,11 @@
       <c r="E33" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>49</v>
       </c>
@@ -3109,8 +3217,11 @@
       <c r="E34" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>523</v>
       </c>
@@ -3126,8 +3237,11 @@
       <c r="E35" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
@@ -3143,8 +3257,11 @@
       <c r="E36" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
@@ -3160,8 +3277,11 @@
       <c r="E37" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
@@ -3177,8 +3297,11 @@
       <c r="E38" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
@@ -3194,8 +3317,11 @@
       <c r="E39" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
@@ -3211,8 +3337,11 @@
       <c r="E40" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
@@ -3228,8 +3357,11 @@
       <c r="E41" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>8</v>
       </c>
@@ -3245,8 +3377,11 @@
       <c r="E42" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>50</v>
       </c>
@@ -3262,8 +3397,11 @@
       <c r="E43" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
@@ -3279,8 +3417,11 @@
       <c r="E44" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>52</v>
       </c>
@@ -3296,8 +3437,11 @@
       <c r="E45" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>53</v>
       </c>
@@ -3313,8 +3457,11 @@
       <c r="E46" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>54</v>
       </c>
@@ -3330,8 +3477,11 @@
       <c r="E47" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>55</v>
       </c>
@@ -3347,8 +3497,11 @@
       <c r="E48" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>56</v>
       </c>
@@ -3364,8 +3517,11 @@
       <c r="E49" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>57</v>
       </c>
@@ -3381,8 +3537,11 @@
       <c r="E50" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>58</v>
       </c>
@@ -3398,8 +3557,11 @@
       <c r="E51" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>59</v>
       </c>
@@ -3415,8 +3577,11 @@
       <c r="E52" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>60</v>
       </c>
@@ -3432,8 +3597,11 @@
       <c r="E53" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>61</v>
       </c>
@@ -3449,8 +3617,11 @@
       <c r="E54" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>62</v>
       </c>
@@ -3466,8 +3637,11 @@
       <c r="E55" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>64</v>
       </c>
@@ -3483,8 +3657,11 @@
       <c r="E56" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>65</v>
       </c>
@@ -3500,8 +3677,11 @@
       <c r="E57" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>66</v>
       </c>
@@ -3517,8 +3697,11 @@
       <c r="E58" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>67</v>
       </c>
@@ -3534,8 +3717,11 @@
       <c r="E59" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>68</v>
       </c>
@@ -3551,8 +3737,11 @@
       <c r="E60" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>69</v>
       </c>
@@ -3568,8 +3757,11 @@
       <c r="E61" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>70</v>
       </c>
@@ -3585,8 +3777,11 @@
       <c r="E62" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>71</v>
       </c>
@@ -3602,8 +3797,11 @@
       <c r="E63" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>72</v>
       </c>
@@ -3618,6 +3816,9 @@
       </c>
       <c r="E64" s="1" t="s">
         <v>270</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>550</v>
       </c>
     </row>
   </sheetData>
@@ -3627,10 +3828,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1DCE64-6270-5B48-B019-637113CB93DD}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3642,7 +3843,7 @@
     <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>530</v>
       </c>
@@ -3658,8 +3859,11 @@
       <c r="E1" s="1" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -3675,8 +3879,11 @@
       <c r="E2">
         <v>29.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3692,8 +3899,11 @@
       <c r="E3">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -3709,8 +3919,11 @@
       <c r="E4">
         <v>26.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -3726,8 +3939,11 @@
       <c r="E5">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -3743,8 +3959,11 @@
       <c r="E6">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -3754,8 +3973,11 @@
       <c r="C7" s="2">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -3765,8 +3987,11 @@
       <c r="C8" s="1">
         <v>8.1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -3776,8 +4001,11 @@
       <c r="C9" s="2">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -3793,8 +4021,11 @@
       <c r="E10">
         <v>37.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -3810,8 +4041,11 @@
       <c r="E11">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -3827,8 +4061,11 @@
       <c r="E12">
         <v>38.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -3844,8 +4081,11 @@
       <c r="E13">
         <v>27.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -3861,8 +4101,11 @@
       <c r="E14">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -3878,8 +4121,11 @@
       <c r="E15">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -3889,8 +4135,11 @@
       <c r="C16" s="1">
         <v>12.6</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -3900,8 +4149,11 @@
       <c r="C17" s="1">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -3911,8 +4163,11 @@
       <c r="C18" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -3928,8 +4183,11 @@
       <c r="E19">
         <v>52.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -3945,8 +4203,11 @@
       <c r="E20">
         <v>18.899999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -3962,8 +4223,11 @@
       <c r="E21">
         <v>30.7</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
@@ -3979,8 +4243,11 @@
       <c r="E22">
         <v>16.7</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -3996,8 +4263,11 @@
       <c r="E23">
         <v>31.7</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>37</v>
       </c>
@@ -4007,8 +4277,11 @@
       <c r="C24" s="1">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
@@ -4024,8 +4297,11 @@
       <c r="E25">
         <v>45.7</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>39</v>
       </c>
@@ -4041,8 +4317,11 @@
       <c r="E26">
         <v>28.2</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
@@ -4058,8 +4337,11 @@
       <c r="E27">
         <v>42.6</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>41</v>
       </c>
@@ -4075,8 +4357,11 @@
       <c r="E28">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
@@ -4092,8 +4377,11 @@
       <c r="E29">
         <v>14.3</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
@@ -4109,8 +4397,11 @@
       <c r="E30">
         <v>20.6</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>44</v>
       </c>
@@ -4126,8 +4417,11 @@
       <c r="E31">
         <v>57.6</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>45</v>
       </c>
@@ -4137,8 +4431,11 @@
       <c r="C32" s="2">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
@@ -4154,8 +4451,11 @@
       <c r="E33">
         <v>43.2</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>48</v>
       </c>
@@ -4171,8 +4471,11 @@
       <c r="E34">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>49</v>
       </c>
@@ -4188,8 +4491,11 @@
       <c r="E35">
         <v>87.2</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
@@ -4199,8 +4505,11 @@
       <c r="C36" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
@@ -4216,8 +4525,11 @@
       <c r="E37">
         <v>21</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
@@ -4233,8 +4545,11 @@
       <c r="E38">
         <v>11.8</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
@@ -4250,8 +4565,11 @@
       <c r="E39">
         <v>12.9</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
@@ -4267,8 +4585,11 @@
       <c r="E40">
         <v>33</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
@@ -4284,8 +4605,11 @@
       <c r="E41">
         <v>20.2</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>8</v>
       </c>
@@ -4295,8 +4619,11 @@
       <c r="C42" s="1">
         <v>1.4550000000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>50</v>
       </c>
@@ -4312,8 +4639,11 @@
       <c r="E43">
         <v>21.4</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
@@ -4329,8 +4659,11 @@
       <c r="E44">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>52</v>
       </c>
@@ -4346,8 +4679,11 @@
       <c r="E45">
         <v>53</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>53</v>
       </c>
@@ -4363,8 +4699,11 @@
       <c r="E46">
         <v>59.9</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>54</v>
       </c>
@@ -4380,8 +4719,11 @@
       <c r="E47">
         <v>36.6</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>55</v>
       </c>
@@ -4397,8 +4739,11 @@
       <c r="E48">
         <v>22.6</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>56</v>
       </c>
@@ -4414,8 +4759,11 @@
       <c r="E49">
         <v>60.1</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>57</v>
       </c>
@@ -4425,8 +4773,11 @@
       <c r="C50" s="2">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>58</v>
       </c>
@@ -4436,8 +4787,11 @@
       <c r="C51" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>59</v>
       </c>
@@ -4453,8 +4807,11 @@
       <c r="E52">
         <v>41.7</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>60</v>
       </c>
@@ -4470,8 +4827,11 @@
       <c r="E53">
         <v>81.900000000000006</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>61</v>
       </c>
@@ -4487,8 +4847,11 @@
       <c r="E54">
         <v>42</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>62</v>
       </c>
@@ -4504,8 +4867,11 @@
       <c r="E55">
         <v>86.4</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>64</v>
       </c>
@@ -4521,8 +4887,11 @@
       <c r="E56">
         <v>39.700000000000003</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>65</v>
       </c>
@@ -4538,8 +4907,11 @@
       <c r="E57">
         <v>64.7</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>66</v>
       </c>
@@ -4555,8 +4927,11 @@
       <c r="E58">
         <v>20.8</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>67</v>
       </c>
@@ -4572,8 +4947,11 @@
       <c r="E59">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>68</v>
       </c>
@@ -4589,8 +4967,11 @@
       <c r="E60">
         <v>18.600000000000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>69</v>
       </c>
@@ -4600,8 +4981,11 @@
       <c r="C61" s="2">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>70</v>
       </c>
@@ -4611,8 +4995,11 @@
       <c r="C62" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>71</v>
       </c>
@@ -4628,8 +5015,11 @@
       <c r="E63">
         <v>25.9</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>72</v>
       </c>
@@ -4644,6 +5034,9 @@
       </c>
       <c r="E64">
         <v>24.8</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>